<commit_message>
forgot to upload latest changes to warenkorb
</commit_message>
<xml_diff>
--- a/MUH PRE/Product-Sprint-BL.xlsx
+++ b/MUH PRE/Product-Sprint-BL.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Misa\Desktop\SYP_SmartGastro\MUH PRE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PUBLIC\5AHIF\SYP_SmartGastro\MUH PRE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEA52554-4128-4CA6-9B2A-942ACD38A1D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F0075A9-543A-4966-9E16-8E823E83704F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{63ECCBC0-BE6D-DE44-947A-6A12B0328622}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{63ECCBC0-BE6D-DE44-947A-6A12B0328622}"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 1" sheetId="1" r:id="rId1"/>
     <sheet name="Iteration 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Iteration 3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="58">
   <si>
     <t>Product Backlog Gesamt</t>
   </si>
@@ -196,13 +197,25 @@
   </si>
   <si>
     <t>Webapp Posten abhaken wenn gebracht - MIK</t>
+  </si>
+  <si>
+    <t>Product Backlog Iteration 3</t>
+  </si>
+  <si>
+    <t>Product Backlog Iteration 2</t>
+  </si>
+  <si>
+    <t>Prozedur Gesamtpreis - DIZ</t>
+  </si>
+  <si>
+    <t>NoSQL-DB Feedback Option</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -216,8 +229,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -260,8 +287,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -269,11 +302,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -304,6 +348,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -346,8 +405,8 @@
   <autoFilter ref="A1:C42" xr:uid="{8652E4C1-7E60-3A47-A98D-29CA12A4612C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{55A54FF5-C06B-664B-AE1D-26A25C2D71C1}" name="Product Backlog Gesamt"/>
-    <tableColumn id="2" xr3:uid="{694C91D8-E7B3-D440-B4FC-E4D7DD5F6027}" name="Product Backlog Iteration 1"/>
-    <tableColumn id="3" xr3:uid="{012DBECC-49DC-A140-AF7B-D9379E7C693A}" name="Sprint Backlog 1"/>
+    <tableColumn id="2" xr3:uid="{694C91D8-E7B3-D440-B4FC-E4D7DD5F6027}" name="Product Backlog Iteration 2"/>
+    <tableColumn id="3" xr3:uid="{012DBECC-49DC-A140-AF7B-D9379E7C693A}" name="Sprint Backlog 2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -966,8 +1025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4D9DFF8-E0C7-1244-A1AC-850B0A5F8866}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -981,10 +1040,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1244,4 +1303,243 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDF5074D-16F9-46EA-AB45-98B215532C01}">
+  <dimension ref="A1:C35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="58" customWidth="1"/>
+    <col min="2" max="3" width="40.09765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="25"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="25"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="25"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="25"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="25"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="25"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" s="21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" s="21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" s="21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" s="21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" s="18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>